<commit_message>
put old values in folders for tests with new rates
</commit_message>
<xml_diff>
--- a/Data/scenarios.xlsx
+++ b/Data/scenarios.xlsx
@@ -541,94 +541,94 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>0.9752222669676079</v>
+        <v>-0.02344977690475521</v>
       </c>
       <c r="D2" t="n">
-        <v>0.974592732475811</v>
+        <v>-0.02401287342951972</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9739303745271675</v>
+        <v>-0.02460367844594259</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9732325573216779</v>
+        <v>-0.02522428873500645</v>
       </c>
       <c r="G2" t="n">
-        <v>0.972496355082915</v>
+        <v>-0.02587701811145051</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9480117111267026</v>
+        <v>-0.04607133026821583</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9451607102917434</v>
+        <v>-0.04829641013008851</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9419788728931302</v>
+        <v>-0.05074732368792471</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9384050653613198</v>
+        <v>-0.05346029034659393</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9343621034111067</v>
+        <v>-0.05647971215721025</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9558934195187052</v>
+        <v>-0.03398883324524034</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9538582653874711</v>
+        <v>-0.03518472085516693</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9516262150396262</v>
+        <v>-0.03646783132036749</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9491672421420634</v>
+        <v>-0.03784806829059038</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.94644488810716</v>
+        <v>-0.03933689373085549</v>
       </c>
       <c r="R2" t="n">
-        <v>0.9450837958819651</v>
+        <v>-0.0402299362887117</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9418927672262262</v>
+        <v>-0.04191622328075996</v>
       </c>
       <c r="T2" t="n">
-        <v>0.938308016798034</v>
+        <v>-0.04375006058895344</v>
       </c>
       <c r="U2" t="n">
-        <v>0.9342518852045095</v>
+        <v>-0.04575170024679837</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9296248518876704</v>
+        <v>-0.04794527824532811</v>
       </c>
       <c r="W2" t="n">
-        <v>0.9235332609116145</v>
+        <v>-0.05194558063116002</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9172019651864994</v>
+        <v>-0.05479177098899262</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.9097275867734705</v>
+        <v>-0.05796793691303625</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.9007698408413682</v>
+        <v>-0.06153499353629193</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.8898384974057909</v>
+        <v>-0.06556983277209898</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.8751153058703682</v>
+        <v>-0.07141879157394511</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.857293440884999</v>
+        <v>-0.07691173472592662</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.833538258536444</v>
+        <v>-0.08332002216829268</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.8002950197441024</v>
+        <v>-0.09089324975262997</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.7504607984193702</v>
+        <v>-0.09998083253468056</v>
       </c>
     </row>
     <row r="3">
@@ -639,94 +639,94 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>0.977234993531484</v>
+        <v>-0.02061681392379752</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9767046753143286</v>
+        <v>-0.02105081465243104</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9761490599211327</v>
+        <v>-0.02150348043341723</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9755662930405381</v>
+        <v>-0.02197604181866878</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9749543345913381</v>
+        <v>-0.02246983996131749</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9735093534252545</v>
+        <v>-0.02356563498393421</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9727885032829531</v>
+        <v>-0.02413437690053695</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9720273249270385</v>
+        <v>-0.02473125021443375</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9712223367022514</v>
+        <v>-0.0253583950268798</v>
       </c>
       <c r="L3" t="n">
-        <v>0.970369644302599</v>
+        <v>-0.02601817416524011</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9935915212883244</v>
+        <v>-0.002871210767738367</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9935501878041731</v>
+        <v>-0.002879478357002462</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9935083176723245</v>
+        <v>-0.002887793696450693</v>
       </c>
       <c r="P3" t="n">
-        <v>0.9934659003732504</v>
+        <v>-0.002896157200959742</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.993422925110671</v>
+        <v>-0.002904569290225315</v>
       </c>
       <c r="R3" t="n">
-        <v>0.9981928738388598</v>
+        <v>-0.0004932023199460452</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9981896022216725</v>
+        <v>-0.000493445688504383</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9981863187371437</v>
+        <v>-0.0004936892973594364</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9981830233205852</v>
+        <v>-0.0004939331468678456</v>
       </c>
       <c r="V3" t="n">
-        <v>0.998179715906838</v>
+        <v>-0.000494177237385818</v>
       </c>
       <c r="W3" t="n">
-        <v>1.000064697752011</v>
+        <v>9.22018022508354e-05</v>
       </c>
       <c r="X3" t="n">
-        <v>1.000064693566482</v>
+        <v>9.219330186224824e-05</v>
       </c>
       <c r="Y3" t="n">
-        <v>1.000064689381496</v>
+        <v>9.218480304068471e-05</v>
       </c>
       <c r="Z3" t="n">
-        <v>1.00006468519705</v>
+        <v>9.217630578628046e-05</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.000064681013146</v>
+        <v>9.216781009803321e-05</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.000715736228983</v>
+        <v>0.0003759356684309105</v>
       </c>
       <c r="AC3" t="n">
-        <v>1.000715224317028</v>
+        <v>0.0003757943939142417</v>
       </c>
       <c r="AD3" t="n">
-        <v>1.000714713136813</v>
+        <v>0.0003756532255380287</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.00071420268677</v>
+        <v>0.0003755121631827004</v>
       </c>
       <c r="AF3" t="n">
-        <v>1.000713692965337</v>
+        <v>0.0003753712067288651</v>
       </c>
     </row>
     <row r="4">
@@ -737,94 +737,94 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>0.9772349992281624</v>
+        <v>-0.02061681070201453</v>
       </c>
       <c r="D4" t="n">
-        <v>0.97670468127951</v>
+        <v>-0.02105081129357806</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9761490661742582</v>
+        <v>-0.02150347692855677</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9755662996029705</v>
+        <v>-0.02197603815807006</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9749543414866082</v>
+        <v>-0.02246983613436444</v>
       </c>
       <c r="H4" t="n">
-        <v>0.973508221171938</v>
+        <v>-0.0235658541973185</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9727873085692381</v>
+        <v>-0.02413460682281439</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9720260624382672</v>
+        <v>-0.02473149164992727</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9712210005032562</v>
+        <v>-0.02535864886252405</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9703682277444253</v>
+        <v>-0.02601844138146701</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9464545017475714</v>
+        <v>-0.04584840409568143</v>
       </c>
       <c r="N4" t="n">
-        <v>0.9434251745291926</v>
+        <v>-0.04805148814138677</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9400325251029682</v>
+        <v>-0.05047698225565728</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9362070212512452</v>
+        <v>-0.05316035663418557</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.931860179104943</v>
+        <v>-0.05614504737593344</v>
       </c>
       <c r="R4" t="n">
-        <v>0.9245571569606493</v>
+        <v>-0.05735934181845381</v>
       </c>
       <c r="S4" t="n">
-        <v>0.9184011042785519</v>
+        <v>-0.06084963694342027</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9111511350091984</v>
+        <v>-0.06479222000764345</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9024872366647443</v>
+        <v>-0.06928109602357364</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8919510887537574</v>
+        <v>-0.07443826028199856</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8644580090837534</v>
+        <v>-0.09274653274091653</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8432058127844652</v>
+        <v>-0.1022278074297299</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.8140499213379905</v>
+        <v>-0.1138683156771182</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.7715741089239616</v>
+        <v>-0.1285004449018524</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.7039482164654262</v>
+        <v>-0.1474475163528693</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.5917364785441706</v>
+        <v>-0.1748298019548035</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.3100585543411714</v>
+        <v>-0.2118712022913212</v>
       </c>
       <c r="AD4" t="n">
-        <v>-1.22519726032024</v>
+        <v>-0.2688281444699049</v>
       </c>
       <c r="AE4" t="n">
-        <v>-2.816195099667968</v>
+        <v>-0.3676675222612422</v>
       </c>
       <c r="AF4" t="n">
-        <v>-1.644910965111081</v>
+        <v>-0.5814465256885645</v>
       </c>
     </row>
     <row r="5">
@@ -835,94 +835,94 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>0.977233457512824</v>
+        <v>-0.02061559788470009</v>
       </c>
       <c r="D5" t="n">
-        <v>0.976703066895479</v>
+        <v>-0.02104954687880876</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9761473738599268</v>
+        <v>-0.02150215755219915</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9755645235762359</v>
+        <v>-0.02197466015705228</v>
       </c>
       <c r="G5" t="n">
-        <v>0.974952475378883</v>
+        <v>-0.02246839551271851</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9735090144144609</v>
+        <v>-0.02356202124482831</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9727881455710274</v>
+        <v>-0.02413058663988751</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9720269469227554</v>
+        <v>-0.0247272701752187</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9712219366286071</v>
+        <v>-0.02535421059057097</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9703692201688834</v>
+        <v>-0.02601376917242309</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9624409657655305</v>
+        <v>-0.03365416220622304</v>
       </c>
       <c r="N5" t="n">
-        <v>0.9609752332138162</v>
+        <v>-0.0348262090961737</v>
       </c>
       <c r="O5" t="n">
-        <v>0.9593904551986503</v>
+        <v>-0.0360828375411654</v>
       </c>
       <c r="P5" t="n">
-        <v>0.9576715146775761</v>
+        <v>-0.03743354610381923</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.9558006219526382</v>
+        <v>-0.0388893109169757</v>
       </c>
       <c r="R5" t="n">
-        <v>0.9500908909106853</v>
+        <v>-0.04060736109749505</v>
       </c>
       <c r="S5" t="n">
-        <v>0.9474691215684895</v>
+        <v>-0.04232611284567272</v>
       </c>
       <c r="T5" t="n">
-        <v>0.9445566327855116</v>
+        <v>-0.04419679121819036</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9413022308138526</v>
+        <v>-0.04624047169136423</v>
       </c>
       <c r="V5" t="n">
-        <v>0.9376419525369689</v>
+        <v>-0.04848231689319593</v>
       </c>
       <c r="W5" t="n">
-        <v>0.9207925877240718</v>
+        <v>-0.05835984832431593</v>
       </c>
       <c r="X5" t="n">
-        <v>0.9139790943889919</v>
+        <v>-0.06197680528008735</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.9058830709158461</v>
+        <v>-0.06607171936573844</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.8961047710175201</v>
+        <v>-0.07074603129146807</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.8840590605666481</v>
+        <v>-0.07613207333382718</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.8644121972308831</v>
+        <v>-0.08617942711961853</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.8431445053604425</v>
+        <v>-0.09430672680959597</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.8139636875502118</v>
+        <v>-0.1041265620505165</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.7714439657502388</v>
+        <v>-0.1162290984861054</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.703729571560667</v>
+        <v>-0.1315149642141484</v>
       </c>
     </row>
     <row r="6">
@@ -933,94 +933,94 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>0.9724813955922833</v>
+        <v>-0.02616037594671301</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9717026932006687</v>
+        <v>-0.02686312540644958</v>
       </c>
       <c r="E6" t="n">
-        <v>0.970878637059116</v>
+        <v>-0.02760467320454724</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9700051460303055</v>
+        <v>-0.02838832360036028</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9690776341832341</v>
+        <v>-0.0292177670255617</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9424512750110132</v>
+        <v>-0.05011354135718785</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9389371880383798</v>
+        <v>-0.05275740158333174</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9349660310193995</v>
+        <v>-0.05569576544753878</v>
       </c>
       <c r="K6" t="n">
-        <v>0.930442425903224</v>
+        <v>-0.0589807430800466</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9252424737304371</v>
+        <v>-0.06267750914375136</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9389733237392361</v>
+        <v>-0.04717113088490699</v>
       </c>
       <c r="N6" t="n">
-        <v>0.9350070180718876</v>
+        <v>-0.04950640394503952</v>
       </c>
       <c r="O6" t="n">
-        <v>0.9304893111260952</v>
+        <v>-0.0520849421295595</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9252966282978773</v>
+        <v>-0.05494684539200375</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.9192654880418804</v>
+        <v>-0.05814153957805218</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9134818098365735</v>
+        <v>-0.06205188467311738</v>
       </c>
       <c r="S6" t="n">
-        <v>0.9052874515597578</v>
+        <v>-0.06615705459517</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8953784808603522</v>
+        <v>-0.07084387682180356</v>
       </c>
       <c r="U6" t="n">
-        <v>0.8831538602099092</v>
+        <v>-0.07624539628440559</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8676944697243144</v>
+        <v>-0.08253858327495819</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8658532305913077</v>
+        <v>-0.08042473124438186</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8450698517148443</v>
+        <v>-0.08745856263969977</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.8166658673590518</v>
+        <v>-0.09584064795204279</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.7755090056183966</v>
+        <v>-0.1059997308383307</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.710524323050778</v>
+        <v>-0.1185678958885881</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.4816410812216984</v>
+        <v>-0.1718059985881548</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.07623485410228567</v>
+        <v>-0.2074465623939228</v>
       </c>
       <c r="AD6" t="n">
-        <v>-15.11735966147823</v>
+        <v>-0.2617445746251747</v>
       </c>
       <c r="AE6" t="n">
-        <v>-1.933850882535515</v>
+        <v>-0.3545447356411671</v>
       </c>
       <c r="AF6" t="n">
-        <v>-1.482897048044947</v>
+        <v>-0.5492940490513409</v>
       </c>
     </row>
     <row r="7">
@@ -1031,94 +1031,94 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>0.9758332901800706</v>
+        <v>-0.02220016115252152</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9752347966982455</v>
+        <v>-0.02270419800711815</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9746059068179279</v>
+        <v>-0.02323165408141564</v>
       </c>
       <c r="F7" t="n">
-        <v>0.973944244535739</v>
+        <v>-0.02378420039765692</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9732471795891342</v>
+        <v>-0.0243636708270297</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9485970640972241</v>
+        <v>-0.04646504480914875</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9458116223966011</v>
+        <v>-0.04872925167158525</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9427070081184978</v>
+        <v>-0.05122542846735581</v>
       </c>
       <c r="K7" t="n">
-        <v>0.939225028149679</v>
+        <v>-0.05399114816558226</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9352924272364729</v>
+        <v>-0.05707256127771673</v>
       </c>
       <c r="M7" t="n">
-        <v>0.9843063846007321</v>
+        <v>-0.01096836947073912</v>
       </c>
       <c r="N7" t="n">
-        <v>0.9840561682370539</v>
+        <v>-0.01109000878452149</v>
       </c>
       <c r="O7" t="n">
-        <v>0.9837978437841512</v>
+        <v>-0.01121437631638311</v>
       </c>
       <c r="P7" t="n">
-        <v>0.9835310106459195</v>
+        <v>-0.01134156489311114</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.9832552413947122</v>
+        <v>-0.01147167160100641</v>
       </c>
       <c r="R7" t="n">
-        <v>0.9873952239899082</v>
+        <v>-0.007514405846642954</v>
       </c>
       <c r="S7" t="n">
-        <v>0.9872343153948447</v>
+        <v>-0.007571299665113281</v>
       </c>
       <c r="T7" t="n">
-        <v>0.9870692454606891</v>
+        <v>-0.007629061576472239</v>
       </c>
       <c r="U7" t="n">
-        <v>0.9868998506449508</v>
+        <v>-0.007687711601663607</v>
       </c>
       <c r="V7" t="n">
-        <v>0.9867259587216595</v>
+        <v>-0.007747270382060884</v>
       </c>
       <c r="W7" t="n">
-        <v>0.9884891509790024</v>
+        <v>-0.006996024207411306</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9883551083898114</v>
+        <v>-0.007045313390439621</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.9882179071961699</v>
+        <v>-0.007095302016747304</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.9880774344220707</v>
+        <v>-0.007146005081010405</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.9879335716386413</v>
+        <v>-0.007197438009597244</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.9894953860105611</v>
+        <v>-0.006613902959854232</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.9893838676380379</v>
+        <v>-0.006657937915137687</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.9892699560714429</v>
+        <v>-0.006702563164559738</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.9891535734379642</v>
+        <v>-0.006747790657663831</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.9890346384491771</v>
+        <v>-0.006793632668717403</v>
       </c>
     </row>
     <row r="8">
@@ -1129,94 +1129,94 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>0.9728391458120961</v>
+        <v>-0.02602168995290594</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9720808375106749</v>
+        <v>-0.0267169090774185</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9712789704189407</v>
+        <v>-0.02745029614363624</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9704296803948395</v>
+        <v>-0.02822508303153047</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9695286323135448</v>
+        <v>-0.02904487709929878</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9423827287810397</v>
+        <v>-0.04999675967651204</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9388600093578884</v>
+        <v>-0.05262798857347846</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9348784802497586</v>
+        <v>-0.05555155518499324</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9303422625228855</v>
+        <v>-0.05881904458625517</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9251267621786654</v>
+        <v>-0.06249493707657749</v>
       </c>
       <c r="M8" t="n">
-        <v>0.9388186278068957</v>
+        <v>-0.04707652434093104</v>
       </c>
       <c r="N8" t="n">
-        <v>0.9348315314790615</v>
+        <v>-0.04940220861740389</v>
       </c>
       <c r="O8" t="n">
-        <v>0.9302885425592876</v>
+        <v>-0.05196962276290482</v>
       </c>
       <c r="P8" t="n">
-        <v>0.9250646931016357</v>
+        <v>-0.05481852059884745</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.9189945228077889</v>
+        <v>-0.05799787849586219</v>
       </c>
       <c r="R8" t="n">
-        <v>0.9144685853380971</v>
+        <v>-0.06137467986040702</v>
       </c>
       <c r="S8" t="n">
-        <v>0.9064687228919074</v>
+        <v>-0.06538783745070859</v>
       </c>
       <c r="T8" t="n">
-        <v>0.8968179764551613</v>
+        <v>-0.06996253640906373</v>
       </c>
       <c r="U8" t="n">
-        <v>0.8849465262140656</v>
+        <v>-0.07522550343180127</v>
       </c>
       <c r="V8" t="n">
-        <v>0.8699882191999211</v>
+        <v>-0.08134469939532299</v>
       </c>
       <c r="W8" t="n">
-        <v>0.8518340851535848</v>
+        <v>-0.08860758695431899</v>
       </c>
       <c r="X8" t="n">
-        <v>0.8260624722246221</v>
+        <v>-0.09722221261225024</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.7894378044956376</v>
+        <v>-0.1076922959010428</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.7332757637077083</v>
+        <v>-0.1206896403632302</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.6362565770023036</v>
+        <v>-0.1372548828073461</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.4260841301283704</v>
+        <v>-0.1697085398284158</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.3469543437318833</v>
+        <v>-0.2043963451019292</v>
       </c>
       <c r="AD8" t="n">
-        <v>-4.882223606840824</v>
+        <v>-0.2569072475265534</v>
       </c>
       <c r="AE8" t="n">
-        <v>-1.795175297051362</v>
+        <v>-0.3457270262311347</v>
       </c>
       <c r="AF8" t="n">
-        <v>-1.442951336483665</v>
+        <v>-0.5284140413742193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>